<commit_message>
Modif mineures à la demande de Virginie C et Eve
Ajout d'un paragraphe sur les modalités d'inscription en M2.
Ajout d'une mention concernant le calendrier d'alternance
Correction du volume horaire d'un EC
</commit_message>
<xml_diff>
--- a/Maquettes/_SPE_Clean.xlsx
+++ b/Maquettes/_SPE_Clean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="37140" windowHeight="23540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="0" windowWidth="37140" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GEEL" sheetId="1" r:id="rId1"/>
@@ -2181,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="71" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="11" t="s">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="11" t="s">
@@ -5776,7 +5776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mises à jour du 11 juillet
Responsables d'EC et coefficients en ME
</commit_message>
<xml_diff>
--- a/Maquettes/_SPE_Clean.xlsx
+++ b/Maquettes/_SPE_Clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="37140" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="300" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GEEL" sheetId="1" r:id="rId1"/>
     <sheet name="GGL" sheetId="3" r:id="rId2"/>
     <sheet name="GAGL" sheetId="2" r:id="rId3"/>
-    <sheet name="ME" sheetId="4" r:id="rId4"/>
+    <sheet name="MANE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="374">
   <si>
     <t>Semestre 1</t>
   </si>
@@ -1086,9 +1086,6 @@
     <t>L. Checroun</t>
   </si>
   <si>
-    <t>JF. Berthevas</t>
-  </si>
-  <si>
     <t>P. Rambeaud</t>
   </si>
   <si>
@@ -1107,9 +1104,6 @@
     <t>M. Juin</t>
   </si>
   <si>
-    <t>J. Viau</t>
-  </si>
-  <si>
     <t>0,5*M + 0,5*O</t>
   </si>
   <si>
@@ -1147,13 +1141,16 @@
   </si>
   <si>
     <t>SIG pour le littoral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1189,6 +1186,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Athelas Regular"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1250,7 +1252,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1460,8 +1462,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1637,11 +1651,20 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="221">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1746,6 +1769,12 @@
     <cellStyle name="Lien hypertexte" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1850,6 +1879,12 @@
     <cellStyle name="Lien hypertexte visité" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2181,7 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
@@ -3333,7 +3368,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C40" s="12">
         <v>24</v>
@@ -3353,7 +3388,7 @@
         <v>15</v>
       </c>
       <c r="J40" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>53</v>
@@ -3403,26 +3438,26 @@
         <v>15</v>
       </c>
       <c r="J42" s="28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="65" t="s">
+      <c r="A43" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="68"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="7" t="s">
@@ -3790,19 +3825,19 @@
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="65"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="65"/>
-      <c r="F57" s="65"/>
-      <c r="G57" s="65"/>
-      <c r="H57" s="65"/>
-      <c r="I57" s="65"/>
-      <c r="J57" s="65"/>
-      <c r="K57" s="65"/>
+      <c r="B57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="68"/>
+      <c r="J57" s="68"/>
+      <c r="K57" s="68"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="7" t="s">
@@ -4051,7 +4086,7 @@
         <v>15</v>
       </c>
       <c r="J66" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K66" s="12" t="s">
         <v>15</v>
@@ -4062,7 +4097,7 @@
         <v>123</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
@@ -4081,7 +4116,7 @@
         <v>301</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C68" s="12">
         <v>54</v>
@@ -4158,26 +4193,26 @@
       </c>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="65" t="s">
+      <c r="A71" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B71" s="65"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="65"/>
-      <c r="E71" s="65"/>
-      <c r="F71" s="65"/>
-      <c r="G71" s="65"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="65"/>
-      <c r="J71" s="65"/>
-      <c r="K71" s="65"/>
+      <c r="B71" s="68"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
+      <c r="K71" s="68"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C72" s="24"/>
       <c r="D72" s="24"/>
@@ -4221,26 +4256,26 @@
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="65" t="s">
+      <c r="A74" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="B74" s="65"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
-      <c r="K74" s="65"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="68"/>
+      <c r="H74" s="68"/>
+      <c r="I74" s="68"/>
+      <c r="J74" s="68"/>
+      <c r="K74" s="68"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="7" t="s">
         <v>302</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C75" s="24"/>
       <c r="D75" s="24"/>
@@ -4304,7 +4339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
@@ -4546,7 +4581,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>204</v>
@@ -4955,7 +4990,7 @@
         <v>309</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -5330,7 +5365,7 @@
         <v>44</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C36" s="12">
         <v>24</v>
@@ -5350,7 +5385,7 @@
         <v>15</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>53</v>
@@ -5400,7 +5435,7 @@
         <v>15</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>53</v>
@@ -5528,10 +5563,10 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="40" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12">
@@ -5776,8 +5811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="71" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7083,7 +7118,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C47" s="12">
         <v>24</v>
@@ -7103,7 +7138,7 @@
         <v>15</v>
       </c>
       <c r="J47" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K47" s="12" t="s">
         <v>53</v>
@@ -7575,10 +7610,10 @@
         <v>15</v>
       </c>
       <c r="J65" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -7596,8 +7631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7794,9 +7829,7 @@
       <c r="G7" s="56">
         <v>6</v>
       </c>
-      <c r="H7" s="56">
-        <v>2</v>
-      </c>
+      <c r="H7" s="56"/>
       <c r="I7" s="56"/>
       <c r="J7" s="56"/>
       <c r="K7" s="56"/>
@@ -7916,9 +7949,7 @@
       <c r="G11" s="44">
         <v>9</v>
       </c>
-      <c r="H11" s="44">
-        <v>3</v>
-      </c>
+      <c r="H11" s="44"/>
       <c r="I11" s="56"/>
       <c r="J11" s="56"/>
       <c r="K11" s="56"/>
@@ -8036,9 +8067,7 @@
       <c r="G15" s="44">
         <v>9</v>
       </c>
-      <c r="H15" s="44">
-        <v>3</v>
-      </c>
+      <c r="H15" s="44"/>
       <c r="I15" s="56"/>
       <c r="J15" s="56"/>
       <c r="K15" s="56"/>
@@ -8237,9 +8266,7 @@
       <c r="G22" s="56">
         <v>6</v>
       </c>
-      <c r="H22" s="56">
-        <v>2</v>
-      </c>
+      <c r="H22" s="56"/>
       <c r="I22" s="56"/>
       <c r="J22" s="56"/>
       <c r="K22" s="56"/>
@@ -8262,7 +8289,9 @@
       <c r="G23" s="12">
         <v>2</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="67">
+        <v>1</v>
+      </c>
       <c r="I23" s="12" t="s">
         <v>15</v>
       </c>
@@ -8291,7 +8320,9 @@
       <c r="G24" s="12">
         <v>2</v>
       </c>
-      <c r="H24" s="12"/>
+      <c r="H24" s="67">
+        <v>1</v>
+      </c>
       <c r="I24" s="12" t="s">
         <v>15</v>
       </c>
@@ -8322,7 +8353,9 @@
       <c r="G25" s="12">
         <v>2</v>
       </c>
-      <c r="H25" s="12"/>
+      <c r="H25" s="67">
+        <v>1</v>
+      </c>
       <c r="I25" s="12" t="s">
         <v>15</v>
       </c>
@@ -8347,9 +8380,7 @@
       <c r="G26" s="56">
         <v>9</v>
       </c>
-      <c r="H26" s="56">
-        <v>3</v>
-      </c>
+      <c r="H26" s="56"/>
       <c r="I26" s="56"/>
       <c r="J26" s="56"/>
       <c r="K26" s="56"/>
@@ -8465,8 +8496,8 @@
       <c r="G30" s="56">
         <v>6</v>
       </c>
-      <c r="H30" s="56">
-        <v>2</v>
+      <c r="H30" s="56" t="s">
+        <v>373</v>
       </c>
       <c r="I30" s="56"/>
       <c r="J30" s="56"/>
@@ -8487,7 +8518,7 @@
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="37" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="G31" s="17">
         <v>3</v>
@@ -8520,7 +8551,7 @@
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G32" s="17">
         <v>3</v>
@@ -8552,8 +8583,8 @@
       <c r="G33" s="56">
         <v>9</v>
       </c>
-      <c r="H33" s="56">
-        <v>3</v>
+      <c r="H33" s="65">
+        <v>1</v>
       </c>
       <c r="I33" s="56"/>
       <c r="J33" s="56"/>
@@ -8570,13 +8601,13 @@
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="37" t="s">
-        <v>354</v>
+        <v>21</v>
       </c>
       <c r="G34" s="17">
         <v>9</v>
       </c>
-      <c r="H34" s="17">
-        <v>3</v>
+      <c r="H34" s="66">
+        <v>1</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>24</v>
@@ -8597,13 +8628,13 @@
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="37" t="s">
-        <v>354</v>
+        <v>21</v>
       </c>
       <c r="G35" s="17">
         <v>9</v>
       </c>
-      <c r="H35" s="17">
-        <v>3</v>
+      <c r="H35" s="66">
+        <v>1</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>24</v>
@@ -8677,8 +8708,8 @@
       <c r="G38" s="56">
         <v>4</v>
       </c>
-      <c r="H38" s="56">
-        <v>2</v>
+      <c r="H38" s="56" t="s">
+        <v>373</v>
       </c>
       <c r="I38" s="56"/>
       <c r="J38" s="56"/>
@@ -8722,7 +8753,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C40" s="12">
         <v>24</v>
@@ -8742,7 +8773,7 @@
         <v>15</v>
       </c>
       <c r="J40" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>53</v>
@@ -8762,8 +8793,8 @@
       <c r="G41" s="56">
         <v>2</v>
       </c>
-      <c r="H41" s="56">
-        <v>1</v>
+      <c r="H41" s="56" t="s">
+        <v>373</v>
       </c>
       <c r="I41" s="56"/>
       <c r="J41" s="56"/>
@@ -8814,8 +8845,8 @@
       <c r="G43" s="56">
         <v>6</v>
       </c>
-      <c r="H43" s="56">
-        <v>3</v>
+      <c r="H43" s="56" t="s">
+        <v>373</v>
       </c>
       <c r="I43" s="56"/>
       <c r="J43" s="56"/>
@@ -8836,7 +8867,7 @@
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G44" s="17">
         <v>2</v>
@@ -8869,7 +8900,7 @@
       </c>
       <c r="E45" s="17"/>
       <c r="F45" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G45" s="17">
         <v>2</v>
@@ -8902,7 +8933,7 @@
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G46" s="17">
         <v>2</v>
@@ -8934,8 +8965,8 @@
       <c r="G47" s="56">
         <v>6</v>
       </c>
-      <c r="H47" s="56">
-        <v>3</v>
+      <c r="H47" s="65" t="s">
+        <v>373</v>
       </c>
       <c r="I47" s="56"/>
       <c r="J47" s="56"/>
@@ -8956,13 +8987,13 @@
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G48" s="17">
         <v>4</v>
       </c>
-      <c r="H48" s="17">
-        <v>2</v>
+      <c r="H48" s="66">
+        <v>1</v>
       </c>
       <c r="I48" s="17" t="s">
         <v>15</v>
@@ -8989,7 +9020,7 @@
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G49" s="17">
         <v>2</v>
@@ -9021,8 +9052,8 @@
       <c r="G50" s="56">
         <v>6</v>
       </c>
-      <c r="H50" s="56">
-        <v>3</v>
+      <c r="H50" s="56" t="s">
+        <v>373</v>
       </c>
       <c r="I50" s="56"/>
       <c r="J50" s="56"/>
@@ -9076,7 +9107,7 @@
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G52" s="17">
         <v>2</v>
@@ -9109,7 +9140,7 @@
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G53" s="17">
         <v>2</v>
@@ -9141,8 +9172,8 @@
       <c r="G54" s="56">
         <v>6</v>
       </c>
-      <c r="H54" s="56">
-        <v>3</v>
+      <c r="H54" s="65" t="s">
+        <v>373</v>
       </c>
       <c r="I54" s="56"/>
       <c r="J54" s="56"/>
@@ -9163,13 +9194,13 @@
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G55" s="17">
         <v>4</v>
       </c>
-      <c r="H55" s="17">
-        <v>2</v>
+      <c r="H55" s="66">
+        <v>1</v>
       </c>
       <c r="I55" s="17" t="s">
         <v>15</v>
@@ -9196,7 +9227,7 @@
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="37" t="s">
-        <v>361</v>
+        <v>26</v>
       </c>
       <c r="G56" s="17">
         <v>2</v>
@@ -9334,7 +9365,7 @@
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
       <c r="F62" s="37" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G62" s="17">
         <v>30</v>
@@ -9361,7 +9392,7 @@
       <c r="D63" s="17"/>
       <c r="E63" s="17"/>
       <c r="F63" s="37" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G63" s="17">
         <v>30</v>

</xml_diff>

<commit_message>
Modif après conseil UFR Droit-Gestion
</commit_message>
<xml_diff>
--- a/Maquettes/_SPE_Clean.xlsx
+++ b/Maquettes/_SPE_Clean.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500" activeTab="3"/>
@@ -7631,8 +7631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:H35"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9272,9 +9272,7 @@
       <c r="C58" s="17">
         <v>9</v>
       </c>
-      <c r="D58" s="17">
-        <v>24</v>
-      </c>
+      <c r="D58" s="17"/>
       <c r="E58" s="17"/>
       <c r="F58" s="37"/>
       <c r="G58" s="17"/>

</xml_diff>